<commit_message>
first 15 york sites
</commit_message>
<xml_diff>
--- a/data/data_from_M/york/all files.xlsx
+++ b/data/data_from_M/york/all files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindseycovell/Desktop/Spring 2023/Capstone/ehs_capstone_nycdoh/data/data_from_M/york/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1F3B76-5CA9-A54F-89E3-4BC7850178F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EE361F-60CB-524B-8D02-E8F920B6C995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{5C4EB71E-9FBF-A645-9506-0DCF9F00C5E8}"/>
   </bookViews>
@@ -441,7 +441,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,67 +456,67 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2"/>

</xml_diff>

<commit_message>
all files updated to 2/27 with new from M
</commit_message>
<xml_diff>
--- a/data/data_from_M/york/all files.xlsx
+++ b/data/data_from_M/york/all files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindseycovell/Desktop/Spring 2023/Capstone/ehs_capstone_nycdoh/data/data_from_M/york/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EE361F-60CB-524B-8D02-E8F920B6C995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2476860-E2D2-9B45-8DCB-89D8B12B215D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{5C4EB71E-9FBF-A645-9506-0DCF9F00C5E8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>SV 153 Green Street.xlsx</t>
   </si>
@@ -79,6 +79,24 @@
   </si>
   <si>
     <t>SV 1520 Fulton Street.xlsx</t>
+  </si>
+  <si>
+    <t>SV 1127 Flatbush Avenue.xlsx</t>
+  </si>
+  <si>
+    <t>SV 148 West Street.xlsx</t>
+  </si>
+  <si>
+    <t>SV 2501 Pitkin Avenue.xlsx</t>
+  </si>
+  <si>
+    <t>SV 2702 West 15th Street.xlsx</t>
+  </si>
+  <si>
+    <t>SV 432-436 Keap Street.xlsx</t>
+  </si>
+  <si>
+    <t>SV 929 Atlantic Avenue.xlsx</t>
   </si>
 </sst>
 </file>
@@ -438,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329FC5E1-3340-2546-A4CE-F3A5C8681CEC}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,7 +558,35 @@
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
       <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>